<commit_message>
Alterações documentação e PPT Final
</commit_message>
<xml_diff>
--- a/Documentação/Requisitos/MatrizDeRequisitos.xlsx
+++ b/Documentação/Requisitos/MatrizDeRequisitos.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="22130"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\P.I\Documentação\Requisitos\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\NOLE201901\Desktop\projeto\Prove3D\Documentação\Requisitos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F44F793F-B501-467D-8A68-D1A536FD7341}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D41BEC1F-E415-4268-B2F9-5B1985698F29}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="198" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1363" uniqueCount="140">
   <si>
     <t>Proposto</t>
   </si>
@@ -472,12 +472,111 @@
   <si>
     <t>Implementado</t>
   </si>
+  <si>
+    <t>2.0</t>
+  </si>
+  <si>
+    <t>Versão 1.0</t>
+  </si>
+  <si>
+    <t>Lais Silva</t>
+  </si>
+  <si>
+    <t>3.0</t>
+  </si>
+  <si>
+    <t>Versão Final</t>
+  </si>
+  <si>
+    <t>5.3</t>
+  </si>
+  <si>
+    <t>Sistema deverá conter meio de validação</t>
+  </si>
+  <si>
+    <t>Validar usabilidade e corrigir erros</t>
+  </si>
+  <si>
+    <t>lais</t>
+  </si>
+  <si>
+    <t>Validar com cliente a usabilidade</t>
+  </si>
+  <si>
+    <t>Entregue</t>
+  </si>
+  <si>
+    <t>5.4</t>
+  </si>
+  <si>
+    <t>Sistema deverá conter script de instalação</t>
+  </si>
+  <si>
+    <t>5.5</t>
+  </si>
+  <si>
+    <t>Sistema deverá fornecer um KPI</t>
+  </si>
+  <si>
+    <t>Auxiliar na tomada de decisão</t>
+  </si>
+  <si>
+    <t>5.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema deverá ter validações de preenchimento de  campos </t>
+  </si>
+  <si>
+    <t>5.7</t>
+  </si>
+  <si>
+    <t>Sistema deverá conter máscara para cep e telefone</t>
+  </si>
+  <si>
+    <t>Captura de dados</t>
+  </si>
+  <si>
+    <t>Formatação de dados</t>
+  </si>
+  <si>
+    <t>Instalação do sistema</t>
+  </si>
+  <si>
+    <t>media</t>
+  </si>
+  <si>
+    <t>alta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Acesso </t>
+  </si>
+  <si>
+    <t>5.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sistema deverá conter validação de acesso entre as páginas </t>
+  </si>
+  <si>
+    <t>Segurança</t>
+  </si>
+  <si>
+    <t>Instalação aplicação</t>
+  </si>
+  <si>
+    <t>Segurança na aplicação</t>
+  </si>
+  <si>
+    <t>5.8</t>
+  </si>
+  <si>
+    <t>Sistema deverá conter manual de instalação</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="21">
+  <fonts count="22">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -612,8 +711,12 @@
       <sz val="10"/>
       <name val="Exo 2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Arial"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -644,6 +747,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.34998626667073579"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="27">
     <border>
@@ -962,7 +1077,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="74">
+  <cellXfs count="79">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -1079,9 +1194,48 @@
     <xf numFmtId="0" fontId="19" fillId="4" borderId="24" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="15" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1109,33 +1263,6 @@
     <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="14" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="10" fillId="4" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1151,16 +1278,19 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="4" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1663,8 +1793,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D497E6A7-39EC-4CFB-B3D4-EE6510853177}" name="Tabela22" displayName="Tabela22" ref="C7:T21" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
-  <autoFilter ref="C7:T21" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D497E6A7-39EC-4CFB-B3D4-EE6510853177}" name="Tabela22" displayName="Tabela22" ref="C7:T28" totalsRowShown="0" headerRowDxfId="21" dataDxfId="19" headerRowBorderDxfId="20" tableBorderDxfId="18">
+  <autoFilter ref="C7:T28" xr:uid="{00000000-0009-0000-0100-000002000000}"/>
   <tableColumns count="18">
     <tableColumn id="1" xr3:uid="{BE8DC9B1-4A85-4507-BBF2-B072CA9CBE6B}" name="Descrição do Requisito" dataDxfId="17"/>
     <tableColumn id="2" xr3:uid="{340D8D69-B40D-4C74-8B78-D8DDFDB8393F}" name="Objetivo / Estratégia de Negócio" dataDxfId="16"/>
@@ -2013,7 +2143,7 @@
   <dimension ref="B2:E39"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+      <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75"/>
@@ -2028,12 +2158,12 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:5" ht="12.75" customHeight="1">
-      <c r="B2" s="46" t="s">
+      <c r="B2" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="46"/>
-      <c r="D2" s="46"/>
-      <c r="E2" s="46"/>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
     </row>
     <row r="4" spans="2:5" ht="27" customHeight="1">
       <c r="B4" s="6" t="s">
@@ -2060,20 +2190,36 @@
         <v>56</v>
       </c>
       <c r="E5" s="44">
-        <v>43714</v>
+        <v>43712</v>
       </c>
     </row>
     <row r="6" spans="2:5" ht="15">
-      <c r="B6" s="4"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
+      <c r="B6" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E6" s="44">
+        <v>43749</v>
+      </c>
     </row>
     <row r="7" spans="2:5" ht="15">
-      <c r="B7" s="4"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
+      <c r="B7" s="4" t="s">
+        <v>110</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="E7" s="44">
+        <v>43784</v>
+      </c>
     </row>
     <row r="8" spans="2:5" ht="15">
       <c r="B8" s="4"/>
@@ -2134,13 +2280,13 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F02813C6-D354-4033-8248-970AC23D41C2}">
-  <dimension ref="A1:U22"/>
+  <dimension ref="A1:U28"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="66" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="3" ySplit="7" topLeftCell="D8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="7" topLeftCell="K20" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A8" sqref="A8"/>
-      <selection pane="bottomRight" activeCell="U10" sqref="U10"/>
+      <selection pane="bottomRight" activeCell="T33" sqref="T33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -2190,22 +2336,22 @@
       <c r="T1" s="12"/>
     </row>
     <row r="2" spans="1:21" ht="16.5" customHeight="1" thickBot="1">
-      <c r="D2" s="56" t="s">
+      <c r="D2" s="51" t="s">
         <v>20</v>
       </c>
-      <c r="E2" s="57"/>
-      <c r="F2" s="57"/>
-      <c r="G2" s="57"/>
-      <c r="H2" s="57"/>
-      <c r="I2" s="57"/>
-      <c r="J2" s="57"/>
-      <c r="K2" s="57"/>
-      <c r="L2" s="57"/>
-      <c r="M2" s="58"/>
-      <c r="N2" s="62" t="s">
+      <c r="E2" s="52"/>
+      <c r="F2" s="52"/>
+      <c r="G2" s="52"/>
+      <c r="H2" s="52"/>
+      <c r="I2" s="52"/>
+      <c r="J2" s="52"/>
+      <c r="K2" s="52"/>
+      <c r="L2" s="52"/>
+      <c r="M2" s="53"/>
+      <c r="N2" s="57" t="s">
         <v>40</v>
       </c>
-      <c r="O2" s="62"/>
+      <c r="O2" s="57"/>
       <c r="P2" s="7"/>
       <c r="Q2" s="16"/>
       <c r="S2" s="17" t="s">
@@ -2214,42 +2360,42 @@
       <c r="T2" s="12"/>
     </row>
     <row r="3" spans="1:21" ht="14.25" customHeight="1" thickBot="1">
-      <c r="D3" s="59"/>
-      <c r="E3" s="60"/>
-      <c r="F3" s="60"/>
-      <c r="G3" s="60"/>
-      <c r="H3" s="60"/>
-      <c r="I3" s="60"/>
-      <c r="J3" s="60"/>
-      <c r="K3" s="60"/>
-      <c r="L3" s="60"/>
-      <c r="M3" s="61"/>
-      <c r="N3" s="63">
+      <c r="D3" s="54"/>
+      <c r="E3" s="55"/>
+      <c r="F3" s="55"/>
+      <c r="G3" s="55"/>
+      <c r="H3" s="55"/>
+      <c r="I3" s="55"/>
+      <c r="J3" s="55"/>
+      <c r="K3" s="55"/>
+      <c r="L3" s="55"/>
+      <c r="M3" s="56"/>
+      <c r="N3" s="58">
         <v>43712</v>
       </c>
-      <c r="O3" s="64"/>
+      <c r="O3" s="59"/>
       <c r="P3" s="7"/>
       <c r="R3" s="18"/>
       <c r="S3" s="18"/>
       <c r="T3" s="18"/>
     </row>
     <row r="4" spans="1:21" ht="12.75" customHeight="1" thickBot="1">
-      <c r="D4" s="47" t="s">
+      <c r="D4" s="60" t="s">
         <v>42</v>
       </c>
-      <c r="E4" s="48"/>
-      <c r="F4" s="48"/>
-      <c r="G4" s="48"/>
-      <c r="H4" s="48"/>
-      <c r="I4" s="48"/>
-      <c r="J4" s="48"/>
-      <c r="K4" s="48"/>
-      <c r="L4" s="48"/>
-      <c r="M4" s="49"/>
-      <c r="N4" s="65" t="s">
+      <c r="E4" s="61"/>
+      <c r="F4" s="61"/>
+      <c r="G4" s="61"/>
+      <c r="H4" s="61"/>
+      <c r="I4" s="61"/>
+      <c r="J4" s="61"/>
+      <c r="K4" s="61"/>
+      <c r="L4" s="61"/>
+      <c r="M4" s="62"/>
+      <c r="N4" s="69" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="65"/>
+      <c r="O4" s="69"/>
       <c r="P4" s="12"/>
       <c r="R4" s="18"/>
       <c r="S4" s="19"/>
@@ -2258,20 +2404,20 @@
     <row r="5" spans="1:21">
       <c r="A5" s="20"/>
       <c r="C5" s="20"/>
-      <c r="D5" s="50"/>
-      <c r="E5" s="51"/>
-      <c r="F5" s="51"/>
-      <c r="G5" s="51"/>
-      <c r="H5" s="51"/>
-      <c r="I5" s="51"/>
-      <c r="J5" s="51"/>
-      <c r="K5" s="51"/>
-      <c r="L5" s="51"/>
-      <c r="M5" s="52"/>
-      <c r="N5" s="66" t="s">
+      <c r="D5" s="63"/>
+      <c r="E5" s="64"/>
+      <c r="F5" s="64"/>
+      <c r="G5" s="64"/>
+      <c r="H5" s="64"/>
+      <c r="I5" s="64"/>
+      <c r="J5" s="64"/>
+      <c r="K5" s="64"/>
+      <c r="L5" s="64"/>
+      <c r="M5" s="65"/>
+      <c r="N5" s="70" t="s">
         <v>44</v>
       </c>
-      <c r="O5" s="67"/>
+      <c r="O5" s="71"/>
       <c r="P5" s="20"/>
       <c r="R5" s="18"/>
       <c r="S5" s="19"/>
@@ -2279,18 +2425,18 @@
     </row>
     <row r="6" spans="1:21" s="21" customFormat="1" ht="49.5" customHeight="1" thickBot="1">
       <c r="B6" s="22"/>
-      <c r="D6" s="53"/>
-      <c r="E6" s="54"/>
-      <c r="F6" s="54"/>
-      <c r="G6" s="54"/>
-      <c r="H6" s="54"/>
-      <c r="I6" s="54"/>
-      <c r="J6" s="54"/>
-      <c r="K6" s="54"/>
-      <c r="L6" s="54"/>
-      <c r="M6" s="55"/>
-      <c r="N6" s="68"/>
-      <c r="O6" s="69"/>
+      <c r="D6" s="66"/>
+      <c r="E6" s="67"/>
+      <c r="F6" s="67"/>
+      <c r="G6" s="67"/>
+      <c r="H6" s="67"/>
+      <c r="I6" s="67"/>
+      <c r="J6" s="67"/>
+      <c r="K6" s="67"/>
+      <c r="L6" s="67"/>
+      <c r="M6" s="68"/>
+      <c r="N6" s="72"/>
+      <c r="O6" s="73"/>
       <c r="P6" s="23"/>
       <c r="R6" s="24"/>
       <c r="S6" s="24"/>
@@ -2406,7 +2552,7 @@
       <c r="R8" s="35"/>
       <c r="S8" s="37"/>
       <c r="T8" s="35" t="s">
-        <v>106</v>
+        <v>117</v>
       </c>
     </row>
     <row r="9" spans="1:21" s="38" customFormat="1" ht="52.5" customHeight="1">
@@ -2419,7 +2565,9 @@
       <c r="C9" s="33" t="s">
         <v>58</v>
       </c>
-      <c r="D9" s="34"/>
+      <c r="D9" s="34" t="s">
+        <v>132</v>
+      </c>
       <c r="E9" s="35" t="s">
         <v>73</v>
       </c>
@@ -2456,7 +2604,7 @@
       <c r="R9" s="35"/>
       <c r="S9" s="37"/>
       <c r="T9" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="10" spans="1:21" s="38" customFormat="1" ht="53.25" customHeight="1">
@@ -2469,7 +2617,9 @@
       <c r="C10" s="33" t="s">
         <v>72</v>
       </c>
-      <c r="D10" s="34"/>
+      <c r="D10" s="34" t="s">
+        <v>132</v>
+      </c>
       <c r="E10" s="35" t="s">
         <v>73</v>
       </c>
@@ -2506,7 +2656,7 @@
       <c r="R10" s="35"/>
       <c r="S10" s="37"/>
       <c r="T10" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="11" spans="1:21" s="38" customFormat="1" ht="48.75" customHeight="1">
@@ -2558,7 +2708,7 @@
       <c r="R11" s="35"/>
       <c r="S11" s="33"/>
       <c r="T11" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="12" spans="1:21" s="38" customFormat="1" ht="57" customHeight="1">
@@ -2610,7 +2760,7 @@
       <c r="R12" s="35"/>
       <c r="S12" s="33"/>
       <c r="T12" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:21" s="38" customFormat="1" ht="45" customHeight="1">
@@ -2660,7 +2810,7 @@
       <c r="R13" s="35"/>
       <c r="S13" s="33"/>
       <c r="T13" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:21" s="38" customFormat="1" ht="58.5" customHeight="1">
@@ -2712,7 +2862,7 @@
       <c r="R14" s="35"/>
       <c r="S14" s="37"/>
       <c r="T14" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:21" s="38" customFormat="1" ht="58.5" customHeight="1">
@@ -2725,45 +2875,47 @@
       <c r="C15" s="43" t="s">
         <v>95</v>
       </c>
-      <c r="D15" s="70" t="s">
+      <c r="D15" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="E15" s="71" t="s">
+      <c r="E15" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F15" s="71">
+      <c r="F15" s="47">
         <v>1</v>
       </c>
-      <c r="G15" s="71" t="s">
+      <c r="G15" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="H15" s="72" t="s">
+      <c r="H15" s="48" t="s">
         <v>45</v>
       </c>
       <c r="I15" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="J15" s="71" t="s">
+      <c r="J15" s="47" t="s">
         <v>50</v>
       </c>
-      <c r="K15" s="71" t="s">
+      <c r="K15" s="47" t="s">
         <v>53</v>
       </c>
-      <c r="L15" s="71" t="s">
+      <c r="L15" s="47" t="s">
         <v>94</v>
       </c>
       <c r="M15" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="N15" s="73"/>
+      <c r="N15" s="49"/>
       <c r="O15" s="36">
         <v>43712</v>
       </c>
-      <c r="P15" s="71"/>
-      <c r="Q15" s="71"/>
-      <c r="R15" s="71"/>
-      <c r="S15" s="73"/>
-      <c r="T15" s="71"/>
+      <c r="P15" s="47"/>
+      <c r="Q15" s="47"/>
+      <c r="R15" s="47"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="47" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="16" spans="1:21" s="38" customFormat="1" ht="58.5" customHeight="1">
       <c r="A16" s="39" t="s">
@@ -2775,43 +2927,45 @@
       <c r="C16" s="43" t="s">
         <v>96</v>
       </c>
-      <c r="D16" s="70" t="s">
+      <c r="D16" s="46" t="s">
         <v>97</v>
       </c>
-      <c r="E16" s="71" t="s">
+      <c r="E16" s="47" t="s">
         <v>90</v>
       </c>
-      <c r="F16" s="71">
+      <c r="F16" s="47">
         <v>1</v>
       </c>
-      <c r="G16" s="71" t="s">
+      <c r="G16" s="47" t="s">
         <v>31</v>
       </c>
-      <c r="H16" s="72" t="s">
+      <c r="H16" s="48" t="s">
         <v>45</v>
       </c>
-      <c r="I16" s="71" t="s">
+      <c r="I16" s="47" t="s">
         <v>98</v>
       </c>
-      <c r="J16" s="71" t="s">
+      <c r="J16" s="47" t="s">
         <v>49</v>
       </c>
-      <c r="K16" s="71" t="s">
+      <c r="K16" s="47" t="s">
         <v>55</v>
       </c>
-      <c r="L16" s="71"/>
+      <c r="L16" s="47"/>
       <c r="M16" s="34" t="s">
         <v>87</v>
       </c>
-      <c r="N16" s="73"/>
+      <c r="N16" s="49"/>
       <c r="O16" s="36">
         <v>43712</v>
       </c>
-      <c r="P16" s="71"/>
-      <c r="Q16" s="71"/>
-      <c r="R16" s="71"/>
-      <c r="S16" s="73"/>
-      <c r="T16" s="71"/>
+      <c r="P16" s="47"/>
+      <c r="Q16" s="47"/>
+      <c r="R16" s="47"/>
+      <c r="S16" s="49"/>
+      <c r="T16" s="47" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="17" spans="1:20" s="38" customFormat="1" ht="53.25" customHeight="1">
       <c r="A17" s="39">
@@ -2823,14 +2977,14 @@
       <c r="C17" s="33" t="s">
         <v>59</v>
       </c>
-      <c r="D17" s="70" t="s">
+      <c r="D17" s="46" t="s">
         <v>63</v>
       </c>
       <c r="E17" s="35" t="s">
         <v>60</v>
       </c>
       <c r="F17" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G17" s="35" t="s">
         <v>32</v>
@@ -2853,7 +3007,7 @@
       <c r="M17" s="34"/>
       <c r="N17" s="33"/>
       <c r="O17" s="36">
-        <v>43712</v>
+        <v>43749</v>
       </c>
       <c r="P17" s="35"/>
       <c r="Q17" s="35"/>
@@ -2914,7 +3068,7 @@
       <c r="R18" s="35"/>
       <c r="S18" s="37"/>
       <c r="T18" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="19" spans="1:20" s="38" customFormat="1" ht="42" customHeight="1">
@@ -2934,7 +3088,7 @@
         <v>60</v>
       </c>
       <c r="F19" s="35">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G19" s="35" t="s">
         <v>32</v>
@@ -2961,14 +3115,14 @@
         <v>67</v>
       </c>
       <c r="O19" s="36">
-        <v>43712</v>
+        <v>43749</v>
       </c>
       <c r="P19" s="35"/>
       <c r="Q19" s="35"/>
       <c r="R19" s="35"/>
       <c r="S19" s="37"/>
       <c r="T19" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="20" spans="1:20" s="38" customFormat="1" ht="44.25" customHeight="1">
@@ -3014,15 +3168,13 @@
       <c r="N20" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="O20" s="36">
-        <v>43712</v>
-      </c>
+      <c r="O20" s="76"/>
       <c r="P20" s="35"/>
       <c r="Q20" s="35"/>
       <c r="R20" s="35"/>
       <c r="S20" s="37"/>
       <c r="T20" s="35" t="s">
-        <v>0</v>
+        <v>117</v>
       </c>
     </row>
     <row r="21" spans="1:20" s="38" customFormat="1" ht="44.25" customHeight="1">
@@ -3069,18 +3221,367 @@
         <v>67</v>
       </c>
       <c r="O21" s="36">
-        <v>43712</v>
+        <v>43749</v>
       </c>
       <c r="P21" s="35"/>
       <c r="Q21" s="35"/>
       <c r="R21" s="35"/>
       <c r="S21" s="37"/>
       <c r="T21" s="35" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="22" spans="1:20">
-      <c r="M22" s="12"/>
+        <v>117</v>
+      </c>
+    </row>
+    <row r="22" spans="1:20" s="38" customFormat="1" ht="37.5" customHeight="1">
+      <c r="A22" s="39" t="s">
+        <v>133</v>
+      </c>
+      <c r="B22" s="40"/>
+      <c r="C22" s="43" t="s">
+        <v>121</v>
+      </c>
+      <c r="D22" s="46"/>
+      <c r="E22" s="74" t="s">
+        <v>131</v>
+      </c>
+      <c r="F22" s="47">
+        <v>2</v>
+      </c>
+      <c r="G22" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="H22" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="I22" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="J22" s="74" t="s">
+        <v>50</v>
+      </c>
+      <c r="K22" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="L22" s="74" t="s">
+        <v>122</v>
+      </c>
+      <c r="M22" s="34" t="s">
+        <v>87</v>
+      </c>
+      <c r="N22" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="O22" s="36">
+        <v>43749</v>
+      </c>
+      <c r="P22" s="47"/>
+      <c r="Q22" s="47"/>
+      <c r="R22" s="47"/>
+      <c r="S22" s="49"/>
+      <c r="T22" s="47" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="23" spans="1:20" ht="27" customHeight="1">
+      <c r="A23" s="39" t="s">
+        <v>112</v>
+      </c>
+      <c r="B23" s="40">
+        <v>115</v>
+      </c>
+      <c r="C23" s="43" t="s">
+        <v>113</v>
+      </c>
+      <c r="D23" s="46" t="s">
+        <v>114</v>
+      </c>
+      <c r="E23" s="74" t="s">
+        <v>73</v>
+      </c>
+      <c r="F23" s="74">
+        <v>3</v>
+      </c>
+      <c r="G23" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="H23" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="I23" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="J23" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="K23" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="L23" s="74" t="s">
+        <v>116</v>
+      </c>
+      <c r="M23" s="47"/>
+      <c r="N23" s="74"/>
+      <c r="O23" s="78">
+        <v>43784</v>
+      </c>
+      <c r="P23" s="74"/>
+      <c r="Q23" s="74"/>
+      <c r="R23" s="74"/>
+      <c r="S23" s="49"/>
+      <c r="T23" s="74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="24" spans="1:20" ht="28.5" customHeight="1">
+      <c r="A24" s="39" t="s">
+        <v>118</v>
+      </c>
+      <c r="B24" s="40">
+        <v>116</v>
+      </c>
+      <c r="C24" s="43" t="s">
+        <v>119</v>
+      </c>
+      <c r="D24" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="E24" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F24" s="74">
+        <v>3</v>
+      </c>
+      <c r="G24" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="H24" s="75" t="s">
+        <v>46</v>
+      </c>
+      <c r="I24" s="35" t="s">
+        <v>48</v>
+      </c>
+      <c r="J24" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="K24" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="L24" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="M24" s="74"/>
+      <c r="N24" s="74"/>
+      <c r="O24" s="77">
+        <v>43784</v>
+      </c>
+      <c r="P24" s="74"/>
+      <c r="Q24" s="74"/>
+      <c r="R24" s="74"/>
+      <c r="S24" s="49"/>
+      <c r="T24" s="74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="25" spans="1:20" ht="25.5">
+      <c r="A25" s="39" t="s">
+        <v>120</v>
+      </c>
+      <c r="B25" s="40">
+        <v>117</v>
+      </c>
+      <c r="C25" s="43" t="s">
+        <v>134</v>
+      </c>
+      <c r="D25" s="46" t="s">
+        <v>135</v>
+      </c>
+      <c r="E25" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F25" s="74">
+        <v>3</v>
+      </c>
+      <c r="G25" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="H25" s="75" t="s">
+        <v>45</v>
+      </c>
+      <c r="I25" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="J25" s="74" t="s">
+        <v>49</v>
+      </c>
+      <c r="K25" s="74" t="s">
+        <v>115</v>
+      </c>
+      <c r="L25" s="74" t="s">
+        <v>137</v>
+      </c>
+      <c r="M25" s="74"/>
+      <c r="N25" s="33" t="s">
+        <v>67</v>
+      </c>
+      <c r="O25" s="78">
+        <v>43784</v>
+      </c>
+      <c r="P25" s="74"/>
+      <c r="Q25" s="74"/>
+      <c r="R25" s="74"/>
+      <c r="S25" s="49"/>
+      <c r="T25" s="74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="26" spans="1:20" ht="25.5">
+      <c r="A26" s="39" t="s">
+        <v>123</v>
+      </c>
+      <c r="B26" s="40">
+        <v>118</v>
+      </c>
+      <c r="C26" s="43" t="s">
+        <v>124</v>
+      </c>
+      <c r="D26" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="E26" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="F26" s="74">
+        <v>3</v>
+      </c>
+      <c r="G26" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="H26" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="I26" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="J26" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="K26" s="74" t="s">
+        <v>54</v>
+      </c>
+      <c r="L26" s="74" t="s">
+        <v>127</v>
+      </c>
+      <c r="M26" s="74"/>
+      <c r="N26" s="74"/>
+      <c r="O26" s="77">
+        <v>43784</v>
+      </c>
+      <c r="P26" s="74"/>
+      <c r="Q26" s="74"/>
+      <c r="R26" s="74"/>
+      <c r="S26" s="49"/>
+      <c r="T26" s="74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:20" ht="25.5">
+      <c r="A27" s="39" t="s">
+        <v>125</v>
+      </c>
+      <c r="B27" s="40">
+        <v>119</v>
+      </c>
+      <c r="C27" s="43" t="s">
+        <v>126</v>
+      </c>
+      <c r="D27" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="E27" s="74" t="s">
+        <v>130</v>
+      </c>
+      <c r="F27" s="74">
+        <v>3</v>
+      </c>
+      <c r="G27" s="74" t="s">
+        <v>32</v>
+      </c>
+      <c r="H27" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="I27" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="J27" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="K27" s="74" t="s">
+        <v>55</v>
+      </c>
+      <c r="L27" s="74" t="s">
+        <v>128</v>
+      </c>
+      <c r="M27" s="74"/>
+      <c r="N27" s="74"/>
+      <c r="O27" s="78">
+        <v>43784</v>
+      </c>
+      <c r="P27" s="74"/>
+      <c r="Q27" s="74"/>
+      <c r="R27" s="74"/>
+      <c r="S27" s="49"/>
+      <c r="T27" s="74" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" ht="25.5">
+      <c r="A28" s="39" t="s">
+        <v>138</v>
+      </c>
+      <c r="B28" s="40">
+        <v>120</v>
+      </c>
+      <c r="C28" s="43" t="s">
+        <v>139</v>
+      </c>
+      <c r="D28" s="46" t="s">
+        <v>129</v>
+      </c>
+      <c r="E28" s="74" t="s">
+        <v>45</v>
+      </c>
+      <c r="F28" s="74">
+        <v>3</v>
+      </c>
+      <c r="G28" s="74" t="s">
+        <v>31</v>
+      </c>
+      <c r="H28" s="75" t="s">
+        <v>47</v>
+      </c>
+      <c r="I28" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="J28" s="74" t="s">
+        <v>53</v>
+      </c>
+      <c r="K28" s="74" t="s">
+        <v>52</v>
+      </c>
+      <c r="L28" s="74" t="s">
+        <v>136</v>
+      </c>
+      <c r="M28" s="74"/>
+      <c r="N28" s="74"/>
+      <c r="O28" s="77">
+        <v>43784</v>
+      </c>
+      <c r="P28" s="74"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="74"/>
+      <c r="S28" s="49"/>
+      <c r="T28" s="74" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -3091,15 +3592,16 @@
     <mergeCell ref="N4:O4"/>
     <mergeCell ref="N5:O6"/>
   </mergeCells>
+  <phoneticPr fontId="21" type="noConversion"/>
   <dataValidations count="3">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G21" xr:uid="{BE0AE777-72D2-4B8C-9B46-C8A878D8DA6E}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T8:T28" xr:uid="{653F11EF-42CA-4E4C-B2F4-B058CCE12D3C}">
+      <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8:G28" xr:uid="{BE0AE777-72D2-4B8C-9B46-C8A878D8DA6E}">
       <formula1>$S$1:$S$6</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8:H21" xr:uid="{CC00DFBE-CCFA-461A-BA96-7137AA891C0B}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H26:H28 H8:H24" xr:uid="{CC00DFBE-CCFA-461A-BA96-7137AA891C0B}">
       <formula1>"Máxima,Alta,Média,Baixa,Mínima"</formula1>
-    </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="T8:T21" xr:uid="{653F11EF-42CA-4E4C-B2F4-B058CCE12D3C}">
-      <formula1>"Proposto,Aprovado,Projetado,Implementado,Verificado, Entregue, Eliminado, Rejeitado"</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.78740157480314965" right="0.78740157480314965" top="0.98425196850393704" bottom="0.98425196850393704" header="0.51181102362204722" footer="0.51181102362204722"/>

</xml_diff>